<commit_message>
Extent Report Integration with Screenshot Capturing on Test Failure
</commit_message>
<xml_diff>
--- a/resources/Data/ExcelDataDriven.xlsx
+++ b/resources/Data/ExcelDataDriven.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="25">
   <si>
     <t>TestCases</t>
   </si>
@@ -172,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -198,6 +198,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
@@ -543,7 +555,7 @@
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s" s="25">
+      <c r="G2" t="s" s="40">
         <v>24</v>
       </c>
     </row>
@@ -566,7 +578,7 @@
       <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s" s="26">
+      <c r="G3" t="s" s="41">
         <v>24</v>
       </c>
     </row>
@@ -589,7 +601,7 @@
       <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s" s="27">
+      <c r="G4" t="s" s="42">
         <v>24</v>
       </c>
     </row>
@@ -612,7 +624,7 @@
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" t="s" s="28">
+      <c r="G5" t="s" s="37">
         <v>24</v>
       </c>
     </row>
@@ -635,7 +647,7 @@
       <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s" s="29">
+      <c r="G6" t="s" s="38">
         <v>24</v>
       </c>
     </row>
@@ -658,7 +670,7 @@
       <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G7" t="s" s="30">
+      <c r="G7" t="s" s="39">
         <v>24</v>
       </c>
     </row>

</xml_diff>